<commit_message>
All board display functions working
</commit_message>
<xml_diff>
--- a/Layout.xlsx
+++ b/Layout.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Abigail Moore\Dropbox\School\Y4S\Eclipse workspace\CSCI306ClueGame\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{879DB21A-35F9-4DB2-A893-463979ED370E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B12C275D-AFFF-4ED7-AFE8-DE51718EB5E5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="51480" yWindow="2385" windowWidth="29040" windowHeight="15840" xr2:uid="{F6F51EFF-D608-4409-93FF-4C24C606E718}"/>
+    <workbookView xWindow="51480" yWindow="2730" windowWidth="29040" windowHeight="15840" xr2:uid="{F6F51EFF-D608-4409-93FF-4C24C606E718}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="441" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="441" uniqueCount="23">
   <si>
     <t>E</t>
   </si>
@@ -99,6 +99,9 @@
   </si>
   <si>
     <t>W</t>
+  </si>
+  <si>
+    <t>WS</t>
   </si>
 </sst>
 </file>
@@ -478,7 +481,7 @@
   <dimension ref="A1:V22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S15" sqref="S15"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -644,7 +647,7 @@
         <v>4</v>
       </c>
       <c r="G3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H3" s="1" t="s">
         <v>1</v>
@@ -668,7 +671,7 @@
         <v>2</v>
       </c>
       <c r="O3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="P3" s="1" t="s">
         <v>17</v>
@@ -904,7 +907,7 @@
         <v>21</v>
       </c>
       <c r="C7" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D7" t="s">
         <v>21</v>
@@ -1499,7 +1502,7 @@
         <v>21</v>
       </c>
       <c r="T15" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="U15" t="s">
         <v>21</v>
@@ -1794,7 +1797,7 @@
         <v>6</v>
       </c>
       <c r="E20" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="F20" t="s">
         <v>21</v>
@@ -1827,7 +1830,7 @@
         <v>7</v>
       </c>
       <c r="P20" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="Q20" t="s">
         <v>21</v>

</xml_diff>